<commit_message>
Updating source data; fixing app.py and functions to match new data
</commit_message>
<xml_diff>
--- a/prepare_contacts/data/cleaned_inbound_referrals.xlsx
+++ b/prepare_contacts/data/cleaned_inbound_referrals.xlsx
@@ -52,22 +52,25 @@
     <t>Nicholas Dezes</t>
   </si>
   <si>
+    <t>Michael Fedorczyk</t>
+  </si>
+  <si>
     <t>Gelareh Naenifard</t>
   </si>
   <si>
-    <t>Michael Fedorczyk</t>
+    <t>Pain And Rehab Center Of Maryland - Camp Springs, Md</t>
+  </si>
+  <si>
+    <t>Bethesda Spine And Posture</t>
+  </si>
+  <si>
+    <t>Total Health Family Clinic - District Heights</t>
   </si>
   <si>
     <t>Jonathan C. Nou</t>
   </si>
   <si>
-    <t>Total Health Family Clinic - District Heights</t>
-  </si>
-  <si>
-    <t>Bethesda Spine And Posture</t>
-  </si>
-  <si>
-    <t>Pain And Rehab Center Of Maryland - Camp Springs, Md</t>
+    <t>Mid-Atlantic Spinal Rehab &amp; Chiropractic</t>
   </si>
   <si>
     <t>Absolute Chiropractic Care - Lanham, Md</t>
@@ -76,18 +79,15 @@
     <t>Gary Hardnett</t>
   </si>
   <si>
+    <t>Dunkirk Chiropractic &amp; Wellness Center</t>
+  </si>
+  <si>
+    <t>Rising Health Chiropractic</t>
+  </si>
+  <si>
     <t>Pain And Rehab Center Of Maryland - Capitol Heights</t>
   </si>
   <si>
-    <t>Rising Health Chiropractic</t>
-  </si>
-  <si>
-    <t>Dunkirk Chiropractic &amp; Wellness Center</t>
-  </si>
-  <si>
-    <t>Mid-Atlantic Spinal Rehab &amp; Chiropractic</t>
-  </si>
-  <si>
     <t>Kaizo Health Chiropractic &amp; Rehabilitation - Landover, Md</t>
   </si>
   <si>
@@ -106,25 +106,28 @@
     <t>226 East Lafayette Avenue</t>
   </si>
   <si>
+    <t>12102 Old Line Center</t>
+  </si>
+  <si>
     <t>525 Eastern Ave Ne</t>
   </si>
   <si>
-    <t>12102 Old Line Center</t>
+    <t>5855 Allentown Road</t>
+  </si>
+  <si>
+    <t>4733 Elm Street</t>
+  </si>
+  <si>
+    <t>10020 Southern Maryland Blvd</t>
+  </si>
+  <si>
+    <t>5730-A Silver Hill Road</t>
   </si>
   <si>
     <t>525 Main Street</t>
   </si>
   <si>
-    <t>5730-A Silver Hill Road</t>
-  </si>
-  <si>
-    <t>10020 Southern Maryland Blvd</t>
-  </si>
-  <si>
-    <t>4733 Elm Street</t>
-  </si>
-  <si>
-    <t>5855 Allentown Road</t>
+    <t>4201 Northview Drive</t>
   </si>
   <si>
     <t>9470 Annapolis Road</t>
@@ -133,9 +136,6 @@
     <t>770 Bon Haven Drive</t>
   </si>
   <si>
-    <t>4201 Northview Drive</t>
-  </si>
-  <si>
     <t>4301 Garden City Dr</t>
   </si>
   <si>
@@ -151,31 +151,31 @@
     <t>Baltimore</t>
   </si>
   <si>
+    <t>Waldorf</t>
+  </si>
+  <si>
     <t>Fairmount Heights</t>
   </si>
   <si>
-    <t>Waldorf</t>
+    <t>Camp Springs</t>
+  </si>
+  <si>
+    <t>Bethesda</t>
+  </si>
+  <si>
+    <t>Dunkirk</t>
+  </si>
+  <si>
+    <t>District Heights</t>
   </si>
   <si>
     <t>Laurel</t>
   </si>
   <si>
-    <t>District Heights</t>
-  </si>
-  <si>
-    <t>Dunkirk</t>
-  </si>
-  <si>
-    <t>Bethesda</t>
-  </si>
-  <si>
-    <t>Camp Springs</t>
+    <t>Bowie</t>
   </si>
   <si>
     <t>Annapolis</t>
-  </si>
-  <si>
-    <t>Bowie</t>
   </si>
   <si>
     <t>Landover</t>
@@ -688,7 +688,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>993877820</v>
+        <v>996605630</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -703,7 +703,7 @@
         <v>55</v>
       </c>
       <c r="F7">
-        <v>20743</v>
+        <v>20602</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>996605630</v>
+        <v>993877820</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -726,7 +726,7 @@
         <v>55</v>
       </c>
       <c r="F8">
-        <v>20602</v>
+        <v>20743</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>996589146</v>
+        <v>996576449</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -749,7 +749,7 @@
         <v>55</v>
       </c>
       <c r="F9">
-        <v>20707</v>
+        <v>20746</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>996605668</v>
+        <v>995274400</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -772,7 +772,7 @@
         <v>55</v>
       </c>
       <c r="F10">
-        <v>20747</v>
+        <v>20814</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -783,7 +783,7 @@
         <v>995583451</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>995274400</v>
+        <v>996605668</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -818,7 +818,7 @@
         <v>55</v>
       </c>
       <c r="F12">
-        <v>20814</v>
+        <v>20747</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
-        <v>996576449</v>
+        <v>996589146</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
@@ -841,7 +841,7 @@
         <v>55</v>
       </c>
       <c r="F13">
-        <v>20746</v>
+        <v>20707</v>
       </c>
       <c r="G13">
         <v>3</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>993709552</v>
+        <v>996605665</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -858,13 +858,13 @@
         <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
         <v>55</v>
       </c>
       <c r="F14">
-        <v>20706</v>
+        <v>20716</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>993720264</v>
+        <v>993709552</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
@@ -881,13 +881,13 @@
         <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
         <v>55</v>
       </c>
       <c r="F15">
-        <v>21401</v>
+        <v>20706</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -895,22 +895,22 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>994842782</v>
+        <v>993720264</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
         <v>55</v>
       </c>
       <c r="F16">
-        <v>20743</v>
+        <v>21401</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -918,22 +918,22 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>996192077</v>
+        <v>996356411</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
         <v>55</v>
       </c>
       <c r="F17">
-        <v>20743</v>
+        <v>20754</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -941,22 +941,22 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
-        <v>996356411</v>
+        <v>996192077</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
         <v>55</v>
       </c>
       <c r="F18">
-        <v>20754</v>
+        <v>20743</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -964,22 +964,22 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
-        <v>996605665</v>
+        <v>994842782</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
         <v>55</v>
       </c>
       <c r="F19">
-        <v>20716</v>
+        <v>20743</v>
       </c>
       <c r="G19">
         <v>1</v>

</xml_diff>